<commit_message>
Adding in more Classes for each section to have its oen methods to calculcate the right values
</commit_message>
<xml_diff>
--- a/TEST_1.xlsx
+++ b/TEST_1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="184">
   <si>
     <t xml:space="preserve">OFERTA EASTER 2025 </t>
   </si>
@@ -239,10 +239,13 @@
     <t>WP HEIGHT</t>
   </si>
   <si>
-    <t>WD WIDTH</t>
+    <t>WP WIDTH</t>
   </si>
   <si>
     <t>WP DEPTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WET PACK PRICE </t>
   </si>
   <si>
     <t>PRICE PER BUNCH</t>
@@ -2250,6 +2253,7 @@
     <col customWidth="1" min="23" max="23" width="16.0"/>
     <col customWidth="1" min="29" max="29" width="17.63"/>
     <col customWidth="1" min="30" max="30" width="18.13"/>
+    <col customWidth="1" min="35" max="35" width="14.0"/>
     <col customWidth="1" min="36" max="36" width="14.63"/>
     <col customWidth="1" min="37" max="37" width="25.38"/>
     <col customWidth="1" min="38" max="38" width="17.13"/>
@@ -2566,17 +2570,17 @@
       <c r="AH3" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AI3" s="24" t="s">
-        <v>40</v>
+      <c r="AI3" s="40" t="s">
+        <v>73</v>
       </c>
       <c r="AJ3" s="40" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AK3" s="40" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AL3" s="40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AM3" s="41" t="s">
         <v>44</v>
@@ -2588,29 +2592,29 @@
         <v>46</v>
       </c>
       <c r="AP3" s="54" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AQ3" s="41" t="s">
         <v>47</v>
       </c>
       <c r="AR3" s="54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AS3" s="42"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="55"/>
       <c r="B4" s="56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="59">
         <v>6.0</v>
@@ -2699,7 +2703,7 @@
         <v>8</v>
       </c>
       <c r="AD4" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE4" s="77">
         <f t="shared" ref="AE4:AG4" si="1">S4/$AF$1</f>
@@ -2758,16 +2762,16 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="55"/>
       <c r="B5" s="87" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C5" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" s="89">
         <v>50.0</v>
       </c>
       <c r="E5" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F5" s="59">
         <v>4.93</v>
@@ -2855,7 +2859,7 @@
         <v>10.0</v>
       </c>
       <c r="AD5" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE5" s="77">
         <f t="shared" ref="AE5:AG5" si="14">S5/$AF$1</f>
@@ -2914,16 +2918,16 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="55"/>
       <c r="B6" s="87" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D6" s="89">
         <v>50.0</v>
       </c>
       <c r="E6" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F6" s="59">
         <v>7.64</v>
@@ -3011,7 +3015,7 @@
         <v>10.0</v>
       </c>
       <c r="AD6" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE6" s="77">
         <f t="shared" ref="AE6:AG6" si="23">S6/$AF$1</f>
@@ -3070,16 +3074,16 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="55"/>
       <c r="B7" s="87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D7" s="89">
         <v>50.0</v>
       </c>
       <c r="E7" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F7" s="59">
         <v>6.4</v>
@@ -3167,7 +3171,7 @@
         <v>14.0</v>
       </c>
       <c r="AD7" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE7" s="77">
         <f t="shared" ref="AE7:AG7" si="24">S7/$AF$1</f>
@@ -3226,16 +3230,16 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="55"/>
       <c r="B8" s="87" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D8" s="89">
         <v>50.0</v>
       </c>
       <c r="E8" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F8" s="59">
         <f>(0.38*3)+0.15</f>
@@ -3324,7 +3328,7 @@
         <v>10.0</v>
       </c>
       <c r="AD8" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE8" s="77">
         <v>13.0</v>
@@ -3379,16 +3383,16 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="55"/>
       <c r="B9" s="87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C9" s="88" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D9" s="89">
         <v>50.0</v>
       </c>
       <c r="E9" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F9" s="59">
         <v>0.85</v>
@@ -3476,7 +3480,7 @@
         <v>10.0</v>
       </c>
       <c r="AD9" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE9" s="77">
         <v>13.0</v>
@@ -3531,16 +3535,16 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="55"/>
       <c r="B10" s="97" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C10" s="88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D10" s="89">
         <v>50.0</v>
       </c>
       <c r="E10" s="90" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F10" s="59">
         <f>(0.32*12)+0.15</f>
@@ -3629,7 +3633,7 @@
         <v>10.0</v>
       </c>
       <c r="AD10" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE10" s="77">
         <f t="shared" ref="AE10:AG10" si="26">S10/$AF$1</f>
@@ -3688,16 +3692,16 @@
     <row r="11" ht="19.5" customHeight="1">
       <c r="A11" s="55"/>
       <c r="B11" s="98" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C11" s="88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D11" s="89">
         <v>60.0</v>
       </c>
       <c r="E11" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F11" s="59">
         <v>0.38</v>
@@ -3785,7 +3789,7 @@
         <v>10.0</v>
       </c>
       <c r="AD11" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE11" s="77">
         <f t="shared" ref="AE11:AG11" si="27">S11/$AF$1</f>
@@ -3844,16 +3848,16 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="99" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C12" s="100" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D12" s="101">
         <v>60.0</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F12" s="102">
         <v>3.45</v>
@@ -3942,7 +3946,7 @@
         <v>12</v>
       </c>
       <c r="AD12" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE12" s="77">
         <v>13.0</v>
@@ -3998,16 +4002,16 @@
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="9"/>
       <c r="B13" s="99" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C13" s="100" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D13" s="101">
         <v>60.0</v>
       </c>
       <c r="E13" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F13" s="102">
         <f>0.32*5+0.35*5</f>
@@ -4097,7 +4101,7 @@
         <v>10</v>
       </c>
       <c r="AD13" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE13" s="77">
         <v>13.0</v>
@@ -4153,16 +4157,16 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="55"/>
       <c r="B14" s="87" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C14" s="88" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D14" s="89">
         <v>70.0</v>
       </c>
       <c r="E14" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F14" s="59">
         <v>0.38</v>
@@ -4250,7 +4254,7 @@
         <v>10.0</v>
       </c>
       <c r="AD14" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE14" s="77">
         <f t="shared" ref="AE14:AG14" si="31">S14/$AF$1</f>
@@ -4309,16 +4313,16 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="55"/>
       <c r="B15" s="87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C15" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D15" s="89">
         <v>70.0</v>
       </c>
       <c r="E15" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F15" s="59">
         <v>3.2</v>
@@ -4406,7 +4410,7 @@
         <v>14.0</v>
       </c>
       <c r="AD15" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE15" s="77">
         <f t="shared" ref="AE15:AG15" si="33">S15/$AF$1</f>
@@ -4465,16 +4469,16 @@
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="55"/>
       <c r="B16" s="87" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C16" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D16" s="89">
         <v>60.0</v>
       </c>
       <c r="E16" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F16" s="59">
         <v>0.55</v>
@@ -4562,7 +4566,7 @@
         <v>12.0</v>
       </c>
       <c r="AD16" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE16" s="77">
         <f t="shared" ref="AE16:AG16" si="34">S16/$AF$1</f>
@@ -4621,16 +4625,16 @@
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="55"/>
       <c r="B17" s="87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C17" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D17" s="89">
         <v>60.0</v>
       </c>
       <c r="E17" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="59">
         <v>0.36</v>
@@ -4718,7 +4722,7 @@
         <v>9.0</v>
       </c>
       <c r="AD17" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE17" s="77">
         <f t="shared" ref="AE17:AG17" si="35">S17/$AF$1</f>
@@ -4777,16 +4781,16 @@
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="55"/>
       <c r="B18" s="87" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D18" s="89">
         <v>60.0</v>
       </c>
       <c r="E18" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="59">
         <v>0.32</v>
@@ -4874,7 +4878,7 @@
         <v>8.0</v>
       </c>
       <c r="AD18" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE18" s="77">
         <f t="shared" ref="AE18:AG18" si="36">S18/$AF$1</f>
@@ -4933,16 +4937,16 @@
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="55"/>
       <c r="B19" s="87" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C19" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D19" s="89">
         <v>50.0</v>
       </c>
       <c r="E19" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F19" s="59">
         <v>0.35</v>
@@ -5030,7 +5034,7 @@
         <v>6.0</v>
       </c>
       <c r="AD19" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE19" s="77">
         <f t="shared" ref="AE19:AG19" si="37">S19/$AF$1</f>
@@ -5089,16 +5093,16 @@
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="55"/>
       <c r="B20" s="87" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C20" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D20" s="89">
         <v>60.0</v>
       </c>
       <c r="E20" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="59">
         <v>0.35</v>
@@ -5186,7 +5190,7 @@
         <v>6.0</v>
       </c>
       <c r="AD20" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE20" s="77">
         <f t="shared" ref="AE20:AG20" si="38">S20/$AF$1</f>
@@ -5245,16 +5249,16 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="55"/>
       <c r="B21" s="105" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C21" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D21" s="89">
         <v>60.0</v>
       </c>
       <c r="E21" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F21" s="59">
         <v>0.36</v>
@@ -5342,7 +5346,7 @@
         <v>6.0</v>
       </c>
       <c r="AD21" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE21" s="77">
         <f t="shared" ref="AE21:AG21" si="39">S21/$AF$1</f>
@@ -5401,16 +5405,16 @@
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="55"/>
       <c r="B22" s="105" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C22" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="89">
         <v>60.0</v>
       </c>
       <c r="E22" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F22" s="59">
         <v>0.38</v>
@@ -5498,7 +5502,7 @@
         <v>6.0</v>
       </c>
       <c r="AD22" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE22" s="77">
         <f t="shared" ref="AE22:AG22" si="40">S22/$AF$1</f>
@@ -5557,16 +5561,16 @@
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="55"/>
       <c r="B23" s="105" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C23" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D23" s="89">
         <v>60.0</v>
       </c>
       <c r="E23" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23" s="59">
         <v>0.4</v>
@@ -5654,7 +5658,7 @@
         <v>6.0</v>
       </c>
       <c r="AD23" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE23" s="77">
         <f t="shared" ref="AE23:AG23" si="41">S23/$AF$1</f>
@@ -5713,16 +5717,16 @@
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="9"/>
       <c r="B24" s="106" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C24" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24" s="89">
         <v>60.0</v>
       </c>
       <c r="E24" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F24" s="107">
         <v>0.4</v>
@@ -5810,7 +5814,7 @@
         <v>6.0</v>
       </c>
       <c r="AD24" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE24" s="77">
         <f t="shared" ref="AE24:AG24" si="42">S24/$AF$1</f>
@@ -5869,16 +5873,16 @@
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="110"/>
       <c r="B25" s="111" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C25" s="88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D25" s="89">
         <v>60.0</v>
       </c>
       <c r="E25" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F25" s="107">
         <v>0.4</v>
@@ -5966,7 +5970,7 @@
         <v>6.0</v>
       </c>
       <c r="AD25" s="76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE25" s="77">
         <f t="shared" ref="AE25:AG25" si="43">S25/$AF$1</f>
@@ -16157,7 +16161,7 @@
       <c r="R2" s="122"/>
       <c r="S2" s="122"/>
       <c r="T2" s="123" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="U2" s="124">
         <v>6000.0</v>
@@ -16212,7 +16216,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="129" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G3" s="21" t="s">
         <v>12</v>
@@ -16331,16 +16335,16 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="B4" s="130" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C4" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D4" s="132">
         <v>50.0</v>
       </c>
       <c r="E4" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="133">
         <v>5.3</v>
@@ -16426,7 +16430,7 @@
         <v>10</v>
       </c>
       <c r="AC4" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD4" s="77">
         <f t="shared" ref="AD4:AF4" si="1">R4/$AF$2</f>
@@ -16487,16 +16491,16 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="B5" s="151" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" s="152">
         <v>40.0</v>
       </c>
       <c r="E5" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="59">
         <v>3.5</v>
@@ -16582,7 +16586,7 @@
         <v>18</v>
       </c>
       <c r="AC5" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD5" s="77">
         <f t="shared" ref="AD5:AF5" si="15">R5/$AF$2</f>
@@ -16643,16 +16647,16 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="B6" s="130" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C6" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6" s="156">
         <v>50.0</v>
       </c>
       <c r="E6" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="59">
         <v>8.73</v>
@@ -16737,7 +16741,7 @@
         <v>7</v>
       </c>
       <c r="AC6" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD6" s="77">
         <f t="shared" ref="AD6:AF6" si="24">R6/$AF$2</f>
@@ -16798,16 +16802,16 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="B7" s="151" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C7" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D7" s="158">
         <v>50.0</v>
       </c>
       <c r="E7" s="159" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F7" s="59">
         <v>13.63</v>
@@ -16892,7 +16896,7 @@
         <v>7</v>
       </c>
       <c r="AC7" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD7" s="77">
         <f t="shared" ref="AD7:AF7" si="25">R7/$AF$2</f>
@@ -16953,16 +16957,16 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="B8" s="151" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D8" s="158">
         <v>50.0</v>
       </c>
       <c r="E8" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F8" s="59">
         <v>3.75</v>
@@ -17048,7 +17052,7 @@
         <v>10</v>
       </c>
       <c r="AC8" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD8" s="77">
         <f t="shared" ref="AD8:AF8" si="27">R8/$AF$2</f>
@@ -17109,10 +17113,10 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="B9" s="151" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C9" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D9" s="152">
         <v>50.0</v>
@@ -17201,7 +17205,7 @@
         <v>8</v>
       </c>
       <c r="AC9" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD9" s="77">
         <f t="shared" ref="AD9:AF9" si="29">R9/$AF$2</f>
@@ -17262,16 +17266,16 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="B10" s="151" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C10" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D10" s="152">
         <v>60.0</v>
       </c>
       <c r="E10" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F10" s="161">
         <v>0.9</v>
@@ -17357,7 +17361,7 @@
         <v>25</v>
       </c>
       <c r="AC10" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD10" s="77">
         <f t="shared" ref="AD10:AF10" si="30">R10/$AF$2</f>
@@ -17418,16 +17422,16 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="B11" s="151" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C11" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D11" s="152">
         <v>50.0</v>
       </c>
       <c r="E11" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F11" s="59">
         <v>0.66</v>
@@ -17513,7 +17517,7 @@
         <v>16</v>
       </c>
       <c r="AC11" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD11" s="77">
         <f t="shared" ref="AD11:AF11" si="32">R11/$AF$2</f>
@@ -17574,16 +17578,16 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="B12" s="151" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C12" s="163" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D12" s="152">
         <v>40.0</v>
       </c>
       <c r="E12" s="90" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F12" s="59">
         <v>0.5</v>
@@ -17669,7 +17673,7 @@
         <v>10</v>
       </c>
       <c r="AC12" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD12" s="77">
         <f t="shared" ref="AD12:AF12" si="33">R12/$AF$2</f>
@@ -17730,16 +17734,16 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="151" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C13" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D13" s="152">
         <v>50.0</v>
       </c>
       <c r="E13" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F13" s="59">
         <v>0.55</v>
@@ -17825,7 +17829,7 @@
         <v>10</v>
       </c>
       <c r="AC13" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD13" s="77">
         <f t="shared" ref="AD13:AF13" si="34">R13/$AF$2</f>
@@ -17886,16 +17890,16 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="151" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C14" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D14" s="152">
         <v>50.0</v>
       </c>
       <c r="E14" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F14" s="59">
         <v>0.77</v>
@@ -17981,7 +17985,7 @@
         <v>10</v>
       </c>
       <c r="AC14" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD14" s="77">
         <f t="shared" ref="AD14:AF14" si="35">R14/$AF$2</f>
@@ -18042,16 +18046,16 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="151" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C15" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D15" s="152">
         <v>50.0</v>
       </c>
       <c r="E15" s="90" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F15" s="59">
         <v>7.45</v>
@@ -18137,7 +18141,7 @@
         <v>12</v>
       </c>
       <c r="AC15" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD15" s="77">
         <f t="shared" ref="AD15:AF15" si="36">R15/$AF$2</f>
@@ -18198,16 +18202,16 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="151" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C16" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D16" s="152">
         <v>50.0</v>
       </c>
       <c r="E16" s="90" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F16" s="59">
         <v>0.57</v>
@@ -18293,7 +18297,7 @@
         <v>8</v>
       </c>
       <c r="AC16" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD16" s="77">
         <f t="shared" ref="AD16:AF16" si="37">R16/$AF$2</f>
@@ -18354,16 +18358,16 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="151" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C17" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D17" s="152">
         <v>50.0</v>
       </c>
       <c r="E17" s="90" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F17" s="59">
         <v>0.7</v>
@@ -18449,7 +18453,7 @@
         <v>16</v>
       </c>
       <c r="AC17" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD17" s="77">
         <f t="shared" ref="AD17:AF17" si="38">R17/$AF$2</f>
@@ -18510,7 +18514,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="B18" s="151" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C18" s="166"/>
       <c r="D18" s="152">
@@ -18600,7 +18604,7 @@
         <v>14.0</v>
       </c>
       <c r="AC18" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD18" s="78">
         <v>13.0</v>
@@ -18658,7 +18662,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="B19" s="151" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C19" s="166"/>
       <c r="D19" s="152">
@@ -18748,7 +18752,7 @@
         <v>12.0</v>
       </c>
       <c r="AC19" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD19" s="78">
         <v>13.0</v>
@@ -18806,7 +18810,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="B20" s="151" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C20" s="166"/>
       <c r="D20" s="152">
@@ -18896,7 +18900,7 @@
         <v>14.0</v>
       </c>
       <c r="AC20" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD20" s="78">
         <v>13.0</v>
@@ -18954,16 +18958,16 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="151" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C21" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D21" s="152">
         <v>70.0</v>
       </c>
       <c r="E21" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F21" s="59">
         <v>0.25</v>
@@ -19049,7 +19053,7 @@
         <v>24</v>
       </c>
       <c r="AC21" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD21" s="77">
         <f t="shared" ref="AD21:AF21" si="41">R21/$AF$2</f>
@@ -19110,16 +19114,16 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="151" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C22" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="152">
         <v>60.0</v>
       </c>
       <c r="E22" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F22" s="59">
         <v>0.27</v>
@@ -19205,7 +19209,7 @@
         <v>24</v>
       </c>
       <c r="AC22" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD22" s="77">
         <f t="shared" ref="AD22:AF22" si="45">R22/$AF$2</f>
@@ -19266,16 +19270,16 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="151" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C23" s="131" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D23" s="152">
         <v>60.0</v>
       </c>
       <c r="E23" s="90" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F23" s="59">
         <v>0.26</v>
@@ -19361,7 +19365,7 @@
         <v>24</v>
       </c>
       <c r="AC23" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD23" s="77">
         <f t="shared" ref="AD23:AF23" si="46">R23/$AF$2</f>
@@ -19422,16 +19426,16 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="151" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C24" s="131" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D24" s="152">
         <v>60.0</v>
       </c>
       <c r="E24" s="90" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F24" s="59">
         <v>0.28</v>
@@ -19517,7 +19521,7 @@
         <v>24</v>
       </c>
       <c r="AC24" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD24" s="77">
         <f t="shared" ref="AD24:AF24" si="47">R24/$AF$2</f>
@@ -19578,16 +19582,16 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="B25" s="151" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C25" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D25" s="152">
         <v>70.0</v>
       </c>
       <c r="E25" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F25" s="59">
         <v>0.32</v>
@@ -19673,7 +19677,7 @@
         <v>16</v>
       </c>
       <c r="AC25" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD25" s="77">
         <f t="shared" ref="AD25:AF25" si="48">R25/$AF$2</f>
@@ -19734,16 +19738,16 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="B26" s="151" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C26" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D26" s="152">
         <v>70.0</v>
       </c>
       <c r="E26" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F26" s="59">
         <v>0.35</v>
@@ -19829,7 +19833,7 @@
         <v>20</v>
       </c>
       <c r="AC26" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD26" s="77">
         <f t="shared" ref="AD26:AF26" si="49">R26/$AF$2</f>
@@ -19890,10 +19894,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="151" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C27" s="131" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D27" s="152">
         <v>70.0</v>
@@ -19983,7 +19987,7 @@
         <v>12</v>
       </c>
       <c r="AC27" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD27" s="77">
         <f t="shared" ref="AD27:AF27" si="50">R27/$AF$2</f>
@@ -20044,14 +20048,14 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="151" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C28" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D28" s="171"/>
       <c r="E28" s="90" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F28" s="59">
         <v>1.87</v>
@@ -20137,7 +20141,7 @@
         <v>25</v>
       </c>
       <c r="AC28" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD28" s="77">
         <f t="shared" ref="AD28:AF28" si="51">R28/$AF$2</f>
@@ -20198,16 +20202,16 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="B29" s="151" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C29" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D29" s="158">
         <v>60.0</v>
       </c>
       <c r="E29" s="90" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F29" s="59">
         <v>1.87</v>
@@ -20293,7 +20297,7 @@
         <v>25</v>
       </c>
       <c r="AC29" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD29" s="77">
         <f t="shared" ref="AD29:AF29" si="52">R29/$AF$2</f>
@@ -20354,16 +20358,16 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="151" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C30" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" s="152">
         <v>60.0</v>
       </c>
       <c r="E30" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F30" s="59">
         <v>0.85</v>
@@ -20449,7 +20453,7 @@
         <v>4</v>
       </c>
       <c r="AC30" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD30" s="77">
         <f t="shared" ref="AD30:AF30" si="54">R30/$AF$2</f>
@@ -20510,16 +20514,16 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="151" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C31" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D31" s="152">
         <v>50.0</v>
       </c>
       <c r="E31" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F31" s="59">
         <v>0.6</v>
@@ -20605,7 +20609,7 @@
         <v>4</v>
       </c>
       <c r="AC31" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD31" s="77">
         <f t="shared" ref="AD31:AF31" si="55">R31/$AF$2</f>
@@ -20666,16 +20670,16 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="151" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C32" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D32" s="152">
         <v>60.0</v>
       </c>
       <c r="E32" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F32" s="59">
         <v>0.57</v>
@@ -20761,7 +20765,7 @@
         <v>4</v>
       </c>
       <c r="AC32" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD32" s="77">
         <f t="shared" ref="AD32:AF32" si="56">R32/$AF$2</f>
@@ -20822,16 +20826,16 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="130" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C33" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D33" s="174">
         <v>40.0</v>
       </c>
       <c r="E33" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F33" s="59">
         <v>7.5</v>
@@ -20917,7 +20921,7 @@
         <v>7</v>
       </c>
       <c r="AC33" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD33" s="77">
         <f t="shared" ref="AD33:AF33" si="57">R33/$AF$2</f>
@@ -20978,16 +20982,16 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="151" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C34" s="131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D34" s="152">
         <v>25.0</v>
       </c>
       <c r="E34" s="90" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F34" s="59">
         <v>3.6</v>
@@ -21073,7 +21077,7 @@
         <v>18</v>
       </c>
       <c r="AC34" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD34" s="77">
         <f t="shared" ref="AD34:AF34" si="58">R34/$AF$2</f>
@@ -21134,16 +21138,16 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="151" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C35" s="131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D35" s="152">
         <v>70.0</v>
       </c>
       <c r="E35" s="90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F35" s="59">
         <v>0.99</v>
@@ -21229,7 +21233,7 @@
         <v>4</v>
       </c>
       <c r="AC35" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD35" s="77">
         <f t="shared" ref="AD35:AF35" si="60">R35/$AF$2</f>
@@ -32223,7 +32227,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="175" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B1" s="128" t="s">
         <v>7</v>
@@ -32238,7 +32242,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="129" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>12</v>
@@ -32423,7 +32427,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G3" s="21" t="s">
         <v>12</v>
@@ -32543,16 +32547,16 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="187"/>
       <c r="B4" s="188" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C4" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D4" s="101">
         <v>50.0</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" s="102">
         <v>5.76</v>
@@ -32641,7 +32645,7 @@
         <v>8</v>
       </c>
       <c r="AD4" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE4" s="77">
         <f t="shared" ref="AE4:AG4" si="1">S4/$AF$2</f>
@@ -32699,16 +32703,16 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="187"/>
       <c r="B5" s="188" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C5" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" s="101">
         <v>50.0</v>
       </c>
       <c r="E5" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F5" s="102">
         <v>8.75</v>
@@ -32797,7 +32801,7 @@
         <v>7</v>
       </c>
       <c r="AD5" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE5" s="77">
         <f t="shared" ref="AE5:AG5" si="16">S5/$AF$2</f>
@@ -32855,16 +32859,16 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="187"/>
       <c r="B6" s="188" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C6" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6" s="101">
         <v>70.0</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6" s="102">
         <v>0.22</v>
@@ -32952,7 +32956,7 @@
         <v>1.0</v>
       </c>
       <c r="AD6" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE6" s="77">
         <f t="shared" ref="AE6:AG6" si="24">S6/$AF$2</f>
@@ -33010,16 +33014,16 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="187"/>
       <c r="B7" s="188" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C7" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D7" s="101">
         <v>80.0</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F7" s="102">
         <v>0.3</v>
@@ -33107,7 +33111,7 @@
         <v>1.0</v>
       </c>
       <c r="AD7" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE7" s="77">
         <f t="shared" ref="AE7:AG7" si="26">S7/$AF$2</f>
@@ -33165,16 +33169,16 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="187"/>
       <c r="B8" s="166" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C8" s="99" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D8" s="190">
         <v>50.0</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F8" s="191">
         <f>(6*0.9)+0.15</f>
@@ -33264,7 +33268,7 @@
         <v>14</v>
       </c>
       <c r="AD8" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE8" s="77">
         <f t="shared" ref="AE8:AG8" si="29">S8/$AF$2</f>
@@ -33322,16 +33326,16 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="187"/>
       <c r="B9" s="166" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C9" s="99" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D9" s="190">
         <v>50.0</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F9" s="191">
         <v>0.38</v>
@@ -33420,7 +33424,7 @@
         <v>20</v>
       </c>
       <c r="AD9" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE9" s="77">
         <f t="shared" ref="AE9:AG9" si="32">S9/$AF$2</f>
@@ -33478,16 +33482,16 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="187"/>
       <c r="B10" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C10" s="101">
         <v>50.0</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F10" s="102">
         <v>0.34</v>
@@ -33576,7 +33580,7 @@
         <v>35</v>
       </c>
       <c r="AD10" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE10" s="77">
         <f t="shared" ref="AE10:AG10" si="35">S10/$AF$2</f>
@@ -33634,16 +33638,16 @@
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="192"/>
       <c r="B11" s="100" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C11" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D11" s="101">
         <v>60.0</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F11" s="102">
         <v>0.35</v>
@@ -33732,7 +33736,7 @@
         <v>25</v>
       </c>
       <c r="AD11" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE11" s="77">
         <f t="shared" ref="AE11:AG11" si="36">S11/$AF$2</f>
@@ -33790,16 +33794,16 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="166"/>
       <c r="B12" s="188" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C12" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D12" s="101">
         <v>60.0</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F12" s="102">
         <v>0.3</v>
@@ -33888,7 +33892,7 @@
         <v>25</v>
       </c>
       <c r="AD12" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE12" s="77">
         <f t="shared" ref="AE12:AG12" si="38">S12/$AF$2</f>
@@ -33946,16 +33950,16 @@
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="192"/>
       <c r="B13" s="188" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C13" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D13" s="101">
         <v>60.0</v>
       </c>
       <c r="E13" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F13" s="102">
         <v>0.48</v>
@@ -34044,7 +34048,7 @@
         <v>25</v>
       </c>
       <c r="AD13" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE13" s="77">
         <f t="shared" ref="AE13:AG13" si="39">S13/$AF$2</f>
@@ -34102,16 +34106,16 @@
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="192"/>
       <c r="B14" s="188" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C14" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D14" s="101">
         <v>60.0</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F14" s="102">
         <v>0.38</v>
@@ -34200,7 +34204,7 @@
         <v>25</v>
       </c>
       <c r="AD14" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE14" s="77">
         <f t="shared" ref="AE14:AG14" si="40">S14/$AF$2</f>
@@ -34258,16 +34262,16 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="192"/>
       <c r="B15" s="188" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C15" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D15" s="101">
         <v>70.0</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F15" s="102">
         <v>0.28</v>
@@ -34356,7 +34360,7 @@
         <v>25</v>
       </c>
       <c r="AD15" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE15" s="77">
         <f t="shared" ref="AE15:AG15" si="41">S15/$AF$2</f>
@@ -34414,16 +34418,16 @@
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="192"/>
       <c r="B16" s="188" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C16" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D16" s="101">
         <v>70.0</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F16" s="102">
         <v>0.35</v>
@@ -34512,7 +34516,7 @@
         <v>25</v>
       </c>
       <c r="AD16" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE16" s="77">
         <f t="shared" ref="AE16:AG16" si="42">S16/$AF$2</f>
@@ -34570,16 +34574,16 @@
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="192"/>
       <c r="B17" s="188" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C17" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D17" s="101">
         <v>70.0</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="102">
         <v>1.33</v>
@@ -34668,7 +34672,7 @@
         <v>25</v>
       </c>
       <c r="AD17" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE17" s="77">
         <f t="shared" ref="AE17:AG17" si="43">S17/$AF$2</f>
@@ -34726,16 +34730,16 @@
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="192"/>
       <c r="B18" s="188" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C18" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D18" s="101">
         <v>70.0</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="102">
         <v>0.23</v>
@@ -34823,7 +34827,7 @@
         <v>1.0</v>
       </c>
       <c r="AD18" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE18" s="77">
         <f t="shared" ref="AE18:AG18" si="44">S18/$AF$2</f>
@@ -34881,16 +34885,16 @@
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="192"/>
       <c r="B19" s="188" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C19" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D19" s="101">
         <v>80.0</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F19" s="102">
         <v>0.27</v>
@@ -34978,7 +34982,7 @@
         <v>1.0</v>
       </c>
       <c r="AD19" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE19" s="77">
         <f t="shared" ref="AE19:AG19" si="46">S19/$AF$2</f>
@@ -35036,16 +35040,16 @@
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="187"/>
       <c r="B20" s="188" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C20" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D20" s="101">
         <v>70.0</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="102">
         <v>0.23</v>
@@ -35133,7 +35137,7 @@
         <v>1.0</v>
       </c>
       <c r="AD20" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE20" s="77">
         <f t="shared" ref="AE20:AG20" si="49">S20/$AF$2</f>
@@ -35191,16 +35195,16 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="187"/>
       <c r="B21" s="188" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C21" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D21" s="101">
         <v>80.0</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F21" s="102">
         <v>0.27</v>
@@ -35288,7 +35292,7 @@
         <v>1.0</v>
       </c>
       <c r="AD21" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE21" s="77">
         <f t="shared" ref="AE21:AG21" si="50">S21/$AF$2</f>
@@ -35346,16 +35350,16 @@
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="187"/>
       <c r="B22" s="166" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C22" s="99" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D22" s="190">
         <v>50.0</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F22" s="191">
         <v>0.33</v>
@@ -35444,7 +35448,7 @@
         <v>100</v>
       </c>
       <c r="AD22" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE22" s="77">
         <f t="shared" ref="AE22:AG22" si="51">S22/$AF$2</f>
@@ -35502,16 +35506,16 @@
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="187"/>
       <c r="B23" s="193" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C23" s="99" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" s="190">
         <v>50.0</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F23" s="191">
         <v>0.35</v>
@@ -35600,7 +35604,7 @@
         <v>14</v>
       </c>
       <c r="AD23" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE23" s="77">
         <f t="shared" ref="AE23:AG23" si="54">S23/$AF$2</f>
@@ -35658,16 +35662,16 @@
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="187"/>
       <c r="B24" s="188" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C24" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24" s="101">
         <v>60.0</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F24" s="102">
         <v>0.28</v>
@@ -35755,7 +35759,7 @@
         <v>1.0</v>
       </c>
       <c r="AD24" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE24" s="77">
         <f t="shared" ref="AE24:AG24" si="57">S24/$AF$2</f>
@@ -35813,16 +35817,16 @@
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="187"/>
       <c r="B25" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C25" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D25" s="101">
         <v>25.0</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F25" s="102">
         <v>0.4</v>
@@ -35911,7 +35915,7 @@
         <v>35</v>
       </c>
       <c r="AD25" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE25" s="77">
         <f t="shared" ref="AE25:AG25" si="58">S25/$AF$2</f>
@@ -35969,16 +35973,16 @@
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="187"/>
       <c r="B26" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C26" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D26" s="101">
         <v>50.0</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F26" s="102">
         <v>0.5</v>
@@ -36067,7 +36071,7 @@
         <v>38</v>
       </c>
       <c r="AD26" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE26" s="77">
         <f t="shared" ref="AE26:AG26" si="60">S26/$AF$2</f>
@@ -36125,16 +36129,16 @@
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="187"/>
       <c r="B27" s="188" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C27" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D27" s="101">
         <v>25.0</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F27" s="102">
         <v>0.45</v>
@@ -36223,7 +36227,7 @@
         <v>38</v>
       </c>
       <c r="AD27" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE27" s="77">
         <f t="shared" ref="AE27:AG27" si="63">S27/$AF$2</f>
@@ -36281,16 +36285,16 @@
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="187"/>
       <c r="B28" s="188" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C28" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D28" s="101">
         <v>50.0</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F28" s="102">
         <v>0.5</v>
@@ -36379,7 +36383,7 @@
         <v>30</v>
       </c>
       <c r="AD28" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE28" s="77">
         <f t="shared" ref="AE28:AG28" si="64">S28/$AF$2</f>
@@ -36437,16 +36441,16 @@
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="187"/>
       <c r="B29" s="188" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C29" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D29" s="101">
         <v>70.0</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F29" s="102">
         <v>0.26</v>
@@ -36535,7 +36539,7 @@
         <v>24</v>
       </c>
       <c r="AD29" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE29" s="77">
         <f t="shared" ref="AE29:AG29" si="65">S29/$AF$2</f>
@@ -36593,16 +36597,16 @@
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="187"/>
       <c r="B30" s="188" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C30" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D30" s="101">
         <v>70.0</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F30" s="102">
         <v>0.35</v>
@@ -36691,7 +36695,7 @@
         <v>24</v>
       </c>
       <c r="AD30" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE30" s="77">
         <f t="shared" ref="AE30:AG30" si="66">S30/$AF$2</f>
@@ -36749,16 +36753,16 @@
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="187"/>
       <c r="B31" s="188" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C31" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D31" s="101">
         <v>50.0</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F31" s="102">
         <f>(0.45*3)+(0.6*3)+0.15</f>
@@ -36848,7 +36852,7 @@
         <v>14</v>
       </c>
       <c r="AD31" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE31" s="77">
         <f t="shared" ref="AE31:AG31" si="67">S31/$AF$2</f>
@@ -36906,16 +36910,16 @@
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="187"/>
       <c r="B32" s="188" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C32" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D32" s="101">
         <v>50.0</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F32" s="102">
         <v>4.65</v>
@@ -37004,7 +37008,7 @@
         <v>12</v>
       </c>
       <c r="AD32" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE32" s="77">
         <f t="shared" ref="AE32:AG32" si="68">S32/$AF$2</f>
@@ -37062,16 +37066,16 @@
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="187"/>
       <c r="B33" s="188" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C33" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D33" s="101">
         <v>50.0</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F33" s="102">
         <v>7.0</v>
@@ -37160,7 +37164,7 @@
         <v>8</v>
       </c>
       <c r="AD33" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE33" s="77">
         <f t="shared" ref="AE33:AG33" si="69">S33/$AF$2</f>
@@ -37218,16 +37222,16 @@
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="187"/>
       <c r="B34" s="188" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C34" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D34" s="101">
         <v>50.0</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F34" s="102">
         <v>5.1</v>
@@ -37316,7 +37320,7 @@
         <v>12</v>
       </c>
       <c r="AD34" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE34" s="77">
         <f t="shared" ref="AE34:AG34" si="70">S34/$AF$2</f>
@@ -37374,16 +37378,16 @@
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="187"/>
       <c r="B35" s="188" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C35" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D35" s="101">
         <v>25.0</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F35" s="102">
         <v>4.5</v>
@@ -37472,7 +37476,7 @@
         <v>18</v>
       </c>
       <c r="AD35" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE35" s="77">
         <f t="shared" ref="AE35:AG35" si="71">S35/$AF$2</f>
@@ -37530,16 +37534,16 @@
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="187"/>
       <c r="B36" s="188" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C36" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D36" s="101">
         <v>25.0</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F36" s="102">
         <v>3.42</v>
@@ -37628,7 +37632,7 @@
         <v>18</v>
       </c>
       <c r="AD36" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE36" s="77">
         <f t="shared" ref="AE36:AG36" si="72">S36/$AF$2</f>
@@ -37686,16 +37690,16 @@
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="187"/>
       <c r="B37" s="188" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C37" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D37" s="101">
         <v>25.0</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F37" s="102">
         <v>4.5</v>
@@ -37784,7 +37788,7 @@
         <v>18</v>
       </c>
       <c r="AD37" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE37" s="77">
         <f t="shared" ref="AE37:AG37" si="73">S37/$AF$2</f>
@@ -37842,16 +37846,16 @@
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="187"/>
       <c r="B38" s="166" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C38" s="99" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D38" s="190">
         <v>50.0</v>
       </c>
       <c r="E38" s="58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F38" s="191">
         <v>0.32</v>
@@ -37940,7 +37944,7 @@
         <v>12</v>
       </c>
       <c r="AD38" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE38" s="77">
         <f t="shared" ref="AE38:AG38" si="74">S38/$AF$2</f>
@@ -37998,16 +38002,16 @@
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="187"/>
       <c r="B39" s="166" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C39" s="99" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D39" s="190">
         <v>50.0</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F39" s="191">
         <v>0.38</v>
@@ -38096,7 +38100,7 @@
         <v>35</v>
       </c>
       <c r="AD39" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE39" s="77">
         <f t="shared" ref="AE39:AG39" si="75">S39/$AF$2</f>
@@ -38154,16 +38158,16 @@
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="187"/>
       <c r="B40" s="188" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C40" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D40" s="101">
         <v>60.0</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F40" s="102">
         <v>0.28</v>
@@ -38251,7 +38255,7 @@
         <v>1.0</v>
       </c>
       <c r="AD40" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE40" s="77">
         <f t="shared" ref="AE40:AG40" si="77">S40/$AF$2</f>
@@ -38309,16 +38313,16 @@
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="187"/>
       <c r="B41" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C41" s="101">
         <v>50.0</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F41" s="102">
         <v>0.34</v>
@@ -38407,7 +38411,7 @@
         <v>35</v>
       </c>
       <c r="AD41" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE41" s="77">
         <f t="shared" ref="AE41:AG41" si="78">S41/$AF$2</f>
@@ -38465,16 +38469,16 @@
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="187"/>
       <c r="B42" s="188" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C42" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D42" s="101">
         <v>50.0</v>
       </c>
       <c r="E42" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F42" s="102">
         <v>0.5</v>
@@ -38563,7 +38567,7 @@
         <v>30</v>
       </c>
       <c r="AD42" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE42" s="77">
         <f t="shared" ref="AE42:AG42" si="80">S42/$AF$2</f>
@@ -38621,16 +38625,16 @@
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="187"/>
       <c r="B43" s="188" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C43" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D43" s="101">
         <v>70.0</v>
       </c>
       <c r="E43" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F43" s="102">
         <v>0.35</v>
@@ -38719,7 +38723,7 @@
         <v>24</v>
       </c>
       <c r="AD43" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE43" s="77">
         <f t="shared" ref="AE43:AG43" si="83">S43/$AF$2</f>
@@ -38777,16 +38781,16 @@
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="166"/>
       <c r="B44" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C44" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D44" s="101">
         <v>70.0</v>
       </c>
       <c r="E44" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F44" s="102">
         <v>0.35</v>
@@ -38875,7 +38879,7 @@
         <v>35</v>
       </c>
       <c r="AD44" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE44" s="77">
         <f t="shared" ref="AE44:AG44" si="84">S44/$AF$2</f>
@@ -38933,16 +38937,16 @@
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="192"/>
       <c r="B45" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C45" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D45" s="101">
         <v>50.0</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F45" s="102">
         <v>0.5</v>
@@ -39031,7 +39035,7 @@
         <v>40</v>
       </c>
       <c r="AD45" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE45" s="77">
         <f t="shared" ref="AE45:AG45" si="85">S45/$AF$2</f>
@@ -39089,16 +39093,16 @@
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="192"/>
       <c r="B46" s="188" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C46" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D46" s="101">
         <v>70.0</v>
       </c>
       <c r="E46" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F46" s="102">
         <v>0.28</v>
@@ -39186,7 +39190,7 @@
         <v>10.0</v>
       </c>
       <c r="AD46" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE46" s="77">
         <f t="shared" ref="AE46:AG46" si="86">S46/$AF$2</f>
@@ -39244,16 +39248,16 @@
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="166"/>
       <c r="B47" s="194" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C47" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D47" s="101">
         <v>60.0</v>
       </c>
       <c r="E47" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F47" s="102">
         <v>0.34</v>
@@ -39341,7 +39345,7 @@
         <v>1.0</v>
       </c>
       <c r="AD47" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE47" s="77">
         <f t="shared" ref="AE47:AG47" si="87">S47/$AF$2</f>
@@ -39399,16 +39403,16 @@
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="187"/>
       <c r="B48" s="188" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C48" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D48" s="101">
         <v>50.0</v>
       </c>
       <c r="E48" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F48" s="102">
         <v>5.76</v>
@@ -39497,7 +39501,7 @@
         <v>8</v>
       </c>
       <c r="AD48" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE48" s="77">
         <f t="shared" ref="AE48:AG48" si="88">S48/$AF$2</f>
@@ -39555,16 +39559,16 @@
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="187"/>
       <c r="B49" s="188" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C49" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D49" s="101">
         <v>50.0</v>
       </c>
       <c r="E49" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F49" s="102">
         <v>8.75</v>
@@ -39653,7 +39657,7 @@
         <v>7</v>
       </c>
       <c r="AD49" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE49" s="77">
         <f t="shared" ref="AE49:AG49" si="90">S49/$AF$2</f>
@@ -39711,16 +39715,16 @@
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="166"/>
       <c r="B50" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C50" s="188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D50" s="101">
         <v>70.0</v>
       </c>
       <c r="E50" s="58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F50" s="102">
         <v>0.35</v>
@@ -39809,7 +39813,7 @@
         <v>16</v>
       </c>
       <c r="AD50" s="76" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AE50" s="77">
         <f t="shared" ref="AE50:AG50" si="93">S50/$AF$2</f>

</xml_diff>